<commit_message>
version 0.0.1 - installation, commissioning, audit, inspection, meter disconnection and reconnection.
</commit_message>
<xml_diff>
--- a/documentation/ireps bible v0.1 230601.xlsx
+++ b/documentation/ireps bible v0.1 230601.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fikile\Documents\swprojects\projects_react\react27-app\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40386281-E895-4441-A403-43539B759EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0A501E-B79E-434A-8006-DE0731CD6BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="supplier data structure" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="erf data structure" sheetId="6" r:id="rId4"/>
     <sheet name="ast data structure" sheetId="5" r:id="rId5"/>
     <sheet name="dictionary" sheetId="2" r:id="rId6"/>
+    <sheet name="ast states" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="279">
   <si>
     <t>Supplier Data Structure</t>
   </si>
@@ -1941,15 +1942,52 @@
       </rPr>
       <t>"</t>
     </r>
+  </si>
+  <si>
+    <t>ast sat</t>
+  </si>
+  <si>
+    <t>suuplier</t>
+  </si>
+  <si>
+    <t>stores</t>
+  </si>
+  <si>
+    <t>checked out</t>
+  </si>
+  <si>
+    <t>field</t>
+  </si>
+  <si>
+    <t>service</t>
+  </si>
+  <si>
+    <t>disconnected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lost </t>
+  </si>
+  <si>
+    <t>retired</t>
+  </si>
+  <si>
+    <t>sold</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2270,135 +2308,165 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2410,45 +2478,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="7"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2753,1370 +2790,1158 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:38" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:38" s="24" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="31" t="s">
+    <row r="2" spans="2:38" s="20" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="33"/>
-      <c r="N2" s="31" t="s">
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="57"/>
+      <c r="N2" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="32"/>
-      <c r="W2" s="32"/>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="32"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="32"/>
-      <c r="AF2" s="32"/>
-      <c r="AG2" s="32"/>
-      <c r="AH2" s="32"/>
-      <c r="AI2" s="32"/>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="33"/>
-    </row>
-    <row r="3" spans="2:38" s="24" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="58"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="31" t="s">
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
+      <c r="Q2" s="56"/>
+      <c r="R2" s="56"/>
+      <c r="S2" s="56"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="56"/>
+      <c r="V2" s="56"/>
+      <c r="W2" s="56"/>
+      <c r="X2" s="56"/>
+      <c r="Y2" s="56"/>
+      <c r="Z2" s="56"/>
+      <c r="AA2" s="56"/>
+      <c r="AB2" s="56"/>
+      <c r="AC2" s="56"/>
+      <c r="AD2" s="56"/>
+      <c r="AE2" s="56"/>
+      <c r="AF2" s="56"/>
+      <c r="AG2" s="56"/>
+      <c r="AH2" s="56"/>
+      <c r="AI2" s="56"/>
+      <c r="AJ2" s="56"/>
+      <c r="AK2" s="56"/>
+      <c r="AL2" s="57"/>
+    </row>
+    <row r="3" spans="2:38" s="20" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="24"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="55" t="s">
         <v>81</v>
       </c>
-      <c r="G3" s="32"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="31" t="s">
+      <c r="G3" s="56"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="55" t="s">
         <v>82</v>
       </c>
-      <c r="J3" s="32"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="60"/>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
-      <c r="P3" s="61"/>
-      <c r="Q3" s="61"/>
-      <c r="R3" s="61"/>
-      <c r="S3" s="61"/>
-      <c r="T3" s="61"/>
-      <c r="U3" s="61"/>
-      <c r="V3" s="61"/>
-      <c r="W3" s="61"/>
-      <c r="X3" s="61"/>
-      <c r="Y3" s="61"/>
-      <c r="Z3" s="61"/>
-      <c r="AA3" s="61"/>
-      <c r="AB3" s="61"/>
-      <c r="AC3" s="61"/>
-      <c r="AD3" s="61"/>
-      <c r="AE3" s="61"/>
-      <c r="AF3" s="61"/>
-      <c r="AG3" s="61"/>
-      <c r="AH3" s="61"/>
-      <c r="AI3" s="61"/>
-      <c r="AJ3" s="61"/>
-      <c r="AK3" s="61"/>
-      <c r="AL3" s="61"/>
-    </row>
-    <row r="4" spans="2:38" s="25" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="26" t="s">
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="26"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="39"/>
+      <c r="Z3" s="39"/>
+      <c r="AA3" s="39"/>
+      <c r="AB3" s="39"/>
+      <c r="AC3" s="39"/>
+      <c r="AD3" s="39"/>
+      <c r="AE3" s="39"/>
+      <c r="AF3" s="39"/>
+      <c r="AG3" s="39"/>
+      <c r="AH3" s="39"/>
+      <c r="AI3" s="39"/>
+      <c r="AJ3" s="39"/>
+      <c r="AK3" s="39"/>
+      <c r="AL3" s="39"/>
+    </row>
+    <row r="4" spans="2:38" s="21" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="29" t="s">
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="30" t="s">
+      <c r="H4" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="I4" s="30" t="s">
+      <c r="I4" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="J4" s="30" t="s">
+      <c r="J4" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30" t="s">
+      <c r="K4" s="23"/>
+      <c r="L4" s="23" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="2:38" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="36"/>
-      <c r="P5" s="36"/>
-      <c r="Q5" s="36"/>
-      <c r="R5" s="36"/>
-      <c r="S5" s="36"/>
-      <c r="T5" s="36"/>
-      <c r="U5" s="36"/>
-      <c r="V5" s="36"/>
-      <c r="W5" s="36"/>
-      <c r="X5" s="36"/>
-      <c r="Y5" s="36"/>
-      <c r="Z5" s="36"/>
-      <c r="AA5" s="36"/>
-      <c r="AB5" s="36"/>
-      <c r="AC5" s="36"/>
-      <c r="AD5" s="36"/>
-      <c r="AE5" s="36"/>
-      <c r="AF5" s="36"/>
-      <c r="AG5" s="36"/>
-      <c r="AH5" s="36"/>
-      <c r="AI5" s="36"/>
-      <c r="AJ5" s="36"/>
-      <c r="AK5" s="36"/>
-      <c r="AL5" s="37"/>
+    <row r="5" spans="2:38" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="29"/>
+      <c r="V5" s="29"/>
+      <c r="W5" s="29"/>
+      <c r="X5" s="29"/>
+      <c r="Y5" s="29"/>
+      <c r="Z5" s="29"/>
+      <c r="AA5" s="29"/>
+      <c r="AB5" s="29"/>
+      <c r="AC5" s="29"/>
+      <c r="AD5" s="29"/>
+      <c r="AE5" s="29"/>
+      <c r="AF5" s="29"/>
+      <c r="AG5" s="29"/>
+      <c r="AH5" s="29"/>
+      <c r="AI5" s="29"/>
+      <c r="AJ5" s="29"/>
+      <c r="AK5" s="29"/>
+      <c r="AL5" s="30"/>
     </row>
     <row r="6" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="J6" s="19" t="b">
+      <c r="J6" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="40" t="s">
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="P6" s="41"/>
-      <c r="Q6" s="41"/>
-      <c r="R6" s="41"/>
-      <c r="S6" s="41"/>
-      <c r="T6" s="41"/>
-      <c r="U6" s="41"/>
-      <c r="V6" s="42"/>
-      <c r="W6" s="39"/>
-      <c r="X6" s="40" t="s">
+      <c r="P6" s="68"/>
+      <c r="Q6" s="68"/>
+      <c r="R6" s="68"/>
+      <c r="S6" s="68"/>
+      <c r="T6" s="68"/>
+      <c r="U6" s="68"/>
+      <c r="V6" s="69"/>
+      <c r="W6" s="32"/>
+      <c r="X6" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="Y6" s="41"/>
-      <c r="Z6" s="42"/>
-      <c r="AB6" s="48" t="s">
+      <c r="Y6" s="68"/>
+      <c r="Z6" s="69"/>
+      <c r="AB6" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="AC6" s="49"/>
-      <c r="AD6" s="49"/>
-      <c r="AE6" s="49"/>
-      <c r="AF6" s="50"/>
-      <c r="AH6" s="46" t="s">
+      <c r="AC6" s="36"/>
+      <c r="AD6" s="36"/>
+      <c r="AE6" s="36"/>
+      <c r="AF6" s="37"/>
+      <c r="AH6" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="AI6" s="47"/>
-      <c r="AJ6" s="39"/>
-      <c r="AK6" s="38" t="s">
+      <c r="AI6" s="34"/>
+      <c r="AJ6" s="32"/>
+      <c r="AK6" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="AL6" s="7"/>
+      <c r="AL6" s="6"/>
     </row>
     <row r="7" spans="2:38" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
+      <c r="E7" s="6"/>
       <c r="F7" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="9"/>
-      <c r="W7" s="9"/>
-      <c r="X7" s="9"/>
-      <c r="Y7" s="9"/>
-      <c r="Z7" s="9"/>
-      <c r="AA7" s="9"/>
-      <c r="AB7" s="9"/>
-      <c r="AC7" s="9"/>
-      <c r="AD7" s="9"/>
-      <c r="AE7" s="9"/>
-      <c r="AF7" s="9"/>
-      <c r="AG7" s="9"/>
-      <c r="AH7" s="9"/>
-      <c r="AI7" s="9"/>
-      <c r="AJ7" s="9"/>
-      <c r="AK7" s="9"/>
-      <c r="AL7" s="10"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="8"/>
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="8"/>
+      <c r="AC7" s="8"/>
+      <c r="AD7" s="8"/>
+      <c r="AE7" s="8"/>
+      <c r="AF7" s="8"/>
+      <c r="AG7" s="8"/>
+      <c r="AH7" s="8"/>
+      <c r="AI7" s="8"/>
+      <c r="AJ7" s="8"/>
+      <c r="AK7" s="8"/>
+      <c r="AL7" s="9"/>
     </row>
     <row r="8" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B8" s="5"/>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
+      <c r="E8" s="6"/>
       <c r="F8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="51"/>
-      <c r="P8" s="51"/>
-      <c r="Q8" s="51"/>
-      <c r="R8" s="51"/>
-      <c r="S8" s="51"/>
-      <c r="T8" s="51"/>
-      <c r="U8" s="51"/>
-      <c r="V8" s="51"/>
-      <c r="W8" s="51"/>
-      <c r="X8" s="51"/>
-      <c r="Y8" s="51"/>
-      <c r="Z8" s="51"/>
-      <c r="AA8" s="51"/>
-      <c r="AB8" s="51"/>
-      <c r="AC8" s="51"/>
-      <c r="AD8" s="51"/>
-      <c r="AE8" s="51"/>
-      <c r="AF8" s="51"/>
-      <c r="AG8" s="51"/>
-      <c r="AH8" s="51"/>
-      <c r="AI8" s="51"/>
-      <c r="AJ8" s="51"/>
-      <c r="AK8" s="51"/>
-      <c r="AL8" s="16"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="38"/>
+      <c r="R8" s="38"/>
+      <c r="S8" s="38"/>
+      <c r="T8" s="38"/>
+      <c r="U8" s="38"/>
+      <c r="V8" s="38"/>
+      <c r="W8" s="38"/>
+      <c r="X8" s="38"/>
+      <c r="Y8" s="38"/>
+      <c r="Z8" s="38"/>
+      <c r="AA8" s="38"/>
+      <c r="AB8" s="38"/>
+      <c r="AC8" s="38"/>
+      <c r="AD8" s="38"/>
+      <c r="AE8" s="38"/>
+      <c r="AF8" s="38"/>
+      <c r="AG8" s="38"/>
+      <c r="AH8" s="38"/>
+      <c r="AI8" s="38"/>
+      <c r="AJ8" s="38"/>
+      <c r="AK8" s="38"/>
+      <c r="AL8" s="15"/>
     </row>
     <row r="9" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B9" s="5"/>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
+      <c r="E9" s="6"/>
       <c r="F9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
       <c r="N9" s="5"/>
-      <c r="O9" s="43" t="s">
+      <c r="O9" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="P9" s="44"/>
-      <c r="Q9" s="44"/>
-      <c r="R9" s="44"/>
-      <c r="S9" s="45"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="43" t="s">
+      <c r="P9" s="59"/>
+      <c r="Q9" s="59"/>
+      <c r="R9" s="59"/>
+      <c r="S9" s="60"/>
+      <c r="U9" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="V9" s="44"/>
-      <c r="W9" s="44"/>
-      <c r="X9" s="44"/>
-      <c r="Y9" s="45"/>
-      <c r="Z9" s="6"/>
-      <c r="AA9" s="43" t="s">
+      <c r="V9" s="59"/>
+      <c r="W9" s="59"/>
+      <c r="X9" s="59"/>
+      <c r="Y9" s="60"/>
+      <c r="AA9" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="AB9" s="44"/>
-      <c r="AC9" s="44"/>
-      <c r="AD9" s="44"/>
-      <c r="AE9" s="45"/>
-      <c r="AF9" s="6"/>
-      <c r="AG9" s="43" t="s">
+      <c r="AB9" s="59"/>
+      <c r="AC9" s="59"/>
+      <c r="AD9" s="59"/>
+      <c r="AE9" s="60"/>
+      <c r="AG9" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="AH9" s="44"/>
-      <c r="AI9" s="44"/>
-      <c r="AJ9" s="44"/>
-      <c r="AK9" s="45"/>
-      <c r="AL9" s="7"/>
+      <c r="AH9" s="59"/>
+      <c r="AI9" s="59"/>
+      <c r="AJ9" s="59"/>
+      <c r="AK9" s="60"/>
+      <c r="AL9" s="6"/>
     </row>
     <row r="10" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B10" s="5"/>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
+      <c r="E10" s="6"/>
       <c r="F10" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="H10" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
       <c r="N10" s="5"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="6"/>
-      <c r="V10" s="6"/>
-      <c r="W10" s="6"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="6"/>
-      <c r="AA10" s="6"/>
-      <c r="AB10" s="6"/>
-      <c r="AC10" s="6"/>
-      <c r="AD10" s="6"/>
-      <c r="AE10" s="6"/>
-      <c r="AF10" s="6"/>
-      <c r="AG10" s="6"/>
-      <c r="AH10" s="6"/>
-      <c r="AI10" s="6"/>
-      <c r="AJ10" s="6"/>
-      <c r="AK10" s="6"/>
-      <c r="AL10" s="7"/>
+      <c r="AL10" s="6"/>
     </row>
     <row r="11" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B11" s="5"/>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
+      <c r="E11" s="6"/>
       <c r="F11" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="19" t="s">
+      <c r="H11" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
       <c r="N11" s="5"/>
-      <c r="O11" s="43" t="s">
+      <c r="O11" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="P11" s="44"/>
-      <c r="Q11" s="44"/>
-      <c r="R11" s="44"/>
-      <c r="S11" s="45"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="43" t="s">
+      <c r="P11" s="59"/>
+      <c r="Q11" s="59"/>
+      <c r="R11" s="59"/>
+      <c r="S11" s="60"/>
+      <c r="U11" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="V11" s="44"/>
-      <c r="W11" s="44"/>
-      <c r="X11" s="44"/>
-      <c r="Y11" s="45"/>
-      <c r="Z11" s="6"/>
-      <c r="AA11" s="43" t="s">
+      <c r="V11" s="59"/>
+      <c r="W11" s="59"/>
+      <c r="X11" s="59"/>
+      <c r="Y11" s="60"/>
+      <c r="AA11" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="AB11" s="44"/>
-      <c r="AC11" s="44"/>
-      <c r="AD11" s="44"/>
-      <c r="AE11" s="45"/>
-      <c r="AF11" s="6"/>
-      <c r="AG11" s="43" t="s">
+      <c r="AB11" s="59"/>
+      <c r="AC11" s="59"/>
+      <c r="AD11" s="59"/>
+      <c r="AE11" s="60"/>
+      <c r="AG11" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="AH11" s="44"/>
-      <c r="AI11" s="44"/>
-      <c r="AJ11" s="44"/>
-      <c r="AK11" s="45"/>
-      <c r="AL11" s="7"/>
+      <c r="AH11" s="59"/>
+      <c r="AI11" s="59"/>
+      <c r="AJ11" s="59"/>
+      <c r="AK11" s="60"/>
+      <c r="AL11" s="6"/>
     </row>
     <row r="12" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
+      <c r="E12" s="6"/>
       <c r="F12" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
       <c r="N12" s="5"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
-      <c r="W12" s="6"/>
-      <c r="X12" s="6"/>
-      <c r="Y12" s="6"/>
-      <c r="Z12" s="6"/>
-      <c r="AA12" s="6"/>
-      <c r="AB12" s="6"/>
-      <c r="AC12" s="6"/>
-      <c r="AD12" s="6"/>
-      <c r="AE12" s="6"/>
-      <c r="AF12" s="6"/>
-      <c r="AG12" s="6"/>
-      <c r="AH12" s="6"/>
-      <c r="AI12" s="6"/>
-      <c r="AJ12" s="6"/>
-      <c r="AK12" s="6"/>
-      <c r="AL12" s="7"/>
+      <c r="AL12" s="6"/>
     </row>
     <row r="13" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
+      <c r="E13" s="6"/>
       <c r="F13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
       <c r="N13" s="5"/>
-      <c r="O13" s="43" t="s">
+      <c r="O13" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="P13" s="44"/>
-      <c r="Q13" s="44"/>
-      <c r="R13" s="44"/>
-      <c r="S13" s="44"/>
-      <c r="T13" s="44"/>
-      <c r="U13" s="44"/>
-      <c r="V13" s="44"/>
-      <c r="W13" s="44"/>
-      <c r="X13" s="44"/>
-      <c r="Y13" s="45"/>
-      <c r="Z13" s="6"/>
-      <c r="AA13" s="43" t="s">
+      <c r="P13" s="59"/>
+      <c r="Q13" s="59"/>
+      <c r="R13" s="59"/>
+      <c r="S13" s="59"/>
+      <c r="T13" s="59"/>
+      <c r="U13" s="59"/>
+      <c r="V13" s="59"/>
+      <c r="W13" s="59"/>
+      <c r="X13" s="59"/>
+      <c r="Y13" s="60"/>
+      <c r="AA13" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="AB13" s="44"/>
-      <c r="AC13" s="44"/>
-      <c r="AD13" s="44"/>
-      <c r="AE13" s="45"/>
-      <c r="AF13" s="6"/>
-      <c r="AG13" s="43" t="s">
+      <c r="AB13" s="59"/>
+      <c r="AC13" s="59"/>
+      <c r="AD13" s="59"/>
+      <c r="AE13" s="60"/>
+      <c r="AG13" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="AH13" s="44"/>
-      <c r="AI13" s="44"/>
-      <c r="AJ13" s="44"/>
-      <c r="AK13" s="45"/>
-      <c r="AL13" s="7"/>
+      <c r="AH13" s="59"/>
+      <c r="AI13" s="59"/>
+      <c r="AJ13" s="59"/>
+      <c r="AK13" s="60"/>
+      <c r="AL13" s="6"/>
     </row>
     <row r="14" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
+      <c r="E14" s="6"/>
       <c r="F14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="19" t="s">
+      <c r="H14" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
       <c r="N14" s="5"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="6"/>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="6"/>
-      <c r="Z14" s="6"/>
-      <c r="AA14" s="6"/>
-      <c r="AB14" s="6"/>
-      <c r="AC14" s="6"/>
-      <c r="AD14" s="6"/>
-      <c r="AE14" s="6"/>
-      <c r="AF14" s="6"/>
-      <c r="AG14" s="6"/>
-      <c r="AH14" s="6"/>
-      <c r="AI14" s="6"/>
-      <c r="AJ14" s="6"/>
-      <c r="AK14" s="6"/>
-      <c r="AL14" s="7"/>
+      <c r="AL14" s="6"/>
     </row>
     <row r="15" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B15" s="5"/>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
+      <c r="E15" s="6"/>
       <c r="F15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="H15" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
       <c r="N15" s="5"/>
-      <c r="O15" s="43" t="s">
+      <c r="O15" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="P15" s="44"/>
-      <c r="Q15" s="44"/>
-      <c r="R15" s="44"/>
-      <c r="S15" s="45"/>
-      <c r="T15" s="6"/>
-      <c r="U15" s="43" t="s">
+      <c r="P15" s="59"/>
+      <c r="Q15" s="59"/>
+      <c r="R15" s="59"/>
+      <c r="S15" s="60"/>
+      <c r="U15" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="V15" s="44"/>
-      <c r="W15" s="44"/>
-      <c r="X15" s="44"/>
-      <c r="Y15" s="45"/>
-      <c r="Z15" s="6"/>
-      <c r="AA15" s="43" t="s">
+      <c r="V15" s="59"/>
+      <c r="W15" s="59"/>
+      <c r="X15" s="59"/>
+      <c r="Y15" s="60"/>
+      <c r="AA15" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="AB15" s="44"/>
-      <c r="AC15" s="44"/>
-      <c r="AD15" s="44"/>
-      <c r="AE15" s="45"/>
-      <c r="AF15" s="6"/>
-      <c r="AG15" s="43" t="s">
+      <c r="AB15" s="59"/>
+      <c r="AC15" s="59"/>
+      <c r="AD15" s="59"/>
+      <c r="AE15" s="60"/>
+      <c r="AG15" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="AH15" s="44"/>
-      <c r="AI15" s="44"/>
-      <c r="AJ15" s="44"/>
-      <c r="AK15" s="45"/>
-      <c r="AL15" s="7"/>
+      <c r="AH15" s="59"/>
+      <c r="AI15" s="59"/>
+      <c r="AJ15" s="59"/>
+      <c r="AK15" s="60"/>
+      <c r="AL15" s="6"/>
     </row>
     <row r="16" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>28</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="G16" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H16" s="19" t="s">
+      <c r="H16" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
       <c r="N16" s="5"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
-      <c r="S16" s="6"/>
-      <c r="T16" s="6"/>
-      <c r="U16" s="6"/>
-      <c r="V16" s="6"/>
-      <c r="W16" s="6"/>
-      <c r="X16" s="6"/>
-      <c r="Y16" s="6"/>
-      <c r="Z16" s="6"/>
-      <c r="AA16" s="6"/>
-      <c r="AB16" s="6"/>
-      <c r="AC16" s="6"/>
-      <c r="AD16" s="6"/>
-      <c r="AE16" s="6"/>
-      <c r="AF16" s="6"/>
-      <c r="AG16" s="6"/>
-      <c r="AH16" s="6"/>
-      <c r="AI16" s="6"/>
-      <c r="AJ16" s="6"/>
-      <c r="AK16" s="6"/>
-      <c r="AL16" s="7"/>
+      <c r="AL16" s="6"/>
     </row>
     <row r="17" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="G17" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H17" s="19" t="s">
+      <c r="H17" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
       <c r="N17" s="5"/>
-      <c r="O17" s="43" t="s">
+      <c r="O17" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="P17" s="44"/>
-      <c r="Q17" s="44"/>
-      <c r="R17" s="44"/>
-      <c r="S17" s="45"/>
-      <c r="T17" s="6"/>
-      <c r="U17" s="43" t="s">
+      <c r="P17" s="59"/>
+      <c r="Q17" s="59"/>
+      <c r="R17" s="59"/>
+      <c r="S17" s="60"/>
+      <c r="U17" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="V17" s="44"/>
-      <c r="W17" s="44"/>
-      <c r="X17" s="44"/>
-      <c r="Y17" s="45"/>
-      <c r="Z17" s="6"/>
-      <c r="AA17" s="43" t="s">
+      <c r="V17" s="59"/>
+      <c r="W17" s="59"/>
+      <c r="X17" s="59"/>
+      <c r="Y17" s="60"/>
+      <c r="AA17" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="AB17" s="44"/>
-      <c r="AC17" s="44"/>
-      <c r="AD17" s="44"/>
-      <c r="AE17" s="45"/>
-      <c r="AF17" s="6"/>
-      <c r="AG17" s="6"/>
-      <c r="AH17" s="6"/>
-      <c r="AI17" s="6"/>
-      <c r="AJ17" s="6"/>
-      <c r="AK17" s="6"/>
-      <c r="AL17" s="7"/>
+      <c r="AB17" s="59"/>
+      <c r="AC17" s="59"/>
+      <c r="AD17" s="59"/>
+      <c r="AE17" s="60"/>
+      <c r="AL17" s="6"/>
     </row>
     <row r="18" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
+      <c r="E18" s="6"/>
       <c r="F18" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="G18" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H18" s="19" t="s">
+      <c r="H18" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
       <c r="N18" s="5"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6"/>
-      <c r="S18" s="6"/>
-      <c r="T18" s="6"/>
-      <c r="U18" s="6"/>
-      <c r="V18" s="6"/>
-      <c r="W18" s="6"/>
-      <c r="X18" s="6"/>
-      <c r="Y18" s="6"/>
-      <c r="Z18" s="6"/>
-      <c r="AA18" s="6"/>
-      <c r="AB18" s="6"/>
-      <c r="AC18" s="6"/>
-      <c r="AD18" s="6"/>
-      <c r="AE18" s="6"/>
-      <c r="AF18" s="6"/>
-      <c r="AG18" s="6"/>
-      <c r="AH18" s="6"/>
-      <c r="AI18" s="6"/>
-      <c r="AJ18" s="6"/>
-      <c r="AK18" s="6"/>
-      <c r="AL18" s="7"/>
+      <c r="AL18" s="6"/>
     </row>
     <row r="19" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B19" s="5"/>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
+      <c r="E19" s="6"/>
       <c r="F19" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="G19" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H19" s="19" t="s">
+      <c r="H19" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
       <c r="N19" s="5"/>
-      <c r="O19" s="43" t="s">
+      <c r="O19" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="P19" s="44"/>
-      <c r="Q19" s="44"/>
-      <c r="R19" s="44"/>
-      <c r="S19" s="44"/>
-      <c r="T19" s="44"/>
-      <c r="U19" s="44"/>
-      <c r="V19" s="44"/>
-      <c r="W19" s="44"/>
-      <c r="X19" s="44"/>
-      <c r="Y19" s="45"/>
-      <c r="Z19" s="6"/>
-      <c r="AA19" s="6"/>
-      <c r="AB19" s="6"/>
-      <c r="AC19" s="6"/>
-      <c r="AD19" s="6"/>
-      <c r="AE19" s="6"/>
-      <c r="AF19" s="6"/>
-      <c r="AG19" s="6"/>
-      <c r="AH19" s="6"/>
-      <c r="AI19" s="6"/>
-      <c r="AJ19" s="6"/>
-      <c r="AK19" s="6"/>
-      <c r="AL19" s="7"/>
+      <c r="P19" s="59"/>
+      <c r="Q19" s="59"/>
+      <c r="R19" s="59"/>
+      <c r="S19" s="59"/>
+      <c r="T19" s="59"/>
+      <c r="U19" s="59"/>
+      <c r="V19" s="59"/>
+      <c r="W19" s="59"/>
+      <c r="X19" s="59"/>
+      <c r="Y19" s="60"/>
+      <c r="AL19" s="6"/>
     </row>
     <row r="20" spans="2:38" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="5"/>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
+      <c r="E20" s="6"/>
       <c r="F20" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="G20" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H20" s="19" t="s">
+      <c r="H20" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
-      <c r="U20" s="9"/>
-      <c r="V20" s="9"/>
-      <c r="W20" s="9"/>
-      <c r="X20" s="9"/>
-      <c r="Y20" s="9"/>
-      <c r="Z20" s="9"/>
-      <c r="AA20" s="9"/>
-      <c r="AB20" s="9"/>
-      <c r="AC20" s="9"/>
-      <c r="AD20" s="9"/>
-      <c r="AE20" s="9"/>
-      <c r="AF20" s="9"/>
-      <c r="AG20" s="9"/>
-      <c r="AH20" s="9"/>
-      <c r="AI20" s="9"/>
-      <c r="AJ20" s="9"/>
-      <c r="AK20" s="9"/>
-      <c r="AL20" s="10"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="8"/>
+      <c r="Y20" s="8"/>
+      <c r="Z20" s="8"/>
+      <c r="AA20" s="8"/>
+      <c r="AB20" s="8"/>
+      <c r="AC20" s="8"/>
+      <c r="AD20" s="8"/>
+      <c r="AE20" s="8"/>
+      <c r="AF20" s="8"/>
+      <c r="AG20" s="8"/>
+      <c r="AH20" s="8"/>
+      <c r="AI20" s="8"/>
+      <c r="AJ20" s="8"/>
+      <c r="AK20" s="8"/>
+      <c r="AL20" s="9"/>
     </row>
     <row r="21" spans="2:38" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="5"/>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
+      <c r="E21" s="6"/>
       <c r="F21" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G21" s="19" t="s">
+      <c r="G21" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H21" s="19" t="s">
+      <c r="H21" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="51"/>
-      <c r="P21" s="51"/>
-      <c r="Q21" s="51"/>
-      <c r="R21" s="51"/>
-      <c r="S21" s="51"/>
-      <c r="T21" s="51"/>
-      <c r="U21" s="51"/>
-      <c r="V21" s="51"/>
-      <c r="W21" s="51"/>
-      <c r="X21" s="51"/>
-      <c r="Y21" s="51"/>
-      <c r="Z21" s="51"/>
-      <c r="AA21" s="51"/>
-      <c r="AB21" s="51"/>
-      <c r="AC21" s="51"/>
-      <c r="AD21" s="51"/>
-      <c r="AE21" s="51"/>
-      <c r="AF21" s="51"/>
-      <c r="AG21" s="51"/>
-      <c r="AH21" s="51"/>
-      <c r="AI21" s="51"/>
-      <c r="AJ21" s="51"/>
-      <c r="AK21" s="51"/>
-      <c r="AL21" s="16"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="38"/>
+      <c r="P21" s="38"/>
+      <c r="Q21" s="38"/>
+      <c r="R21" s="38"/>
+      <c r="S21" s="38"/>
+      <c r="T21" s="38"/>
+      <c r="U21" s="38"/>
+      <c r="V21" s="38"/>
+      <c r="W21" s="38"/>
+      <c r="X21" s="38"/>
+      <c r="Y21" s="38"/>
+      <c r="Z21" s="38"/>
+      <c r="AA21" s="38"/>
+      <c r="AB21" s="38"/>
+      <c r="AC21" s="38"/>
+      <c r="AD21" s="38"/>
+      <c r="AE21" s="38"/>
+      <c r="AF21" s="38"/>
+      <c r="AG21" s="38"/>
+      <c r="AH21" s="38"/>
+      <c r="AI21" s="38"/>
+      <c r="AJ21" s="38"/>
+      <c r="AK21" s="38"/>
+      <c r="AL21" s="15"/>
     </row>
     <row r="22" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
+      <c r="E22" s="6"/>
       <c r="F22" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G22" s="19" t="s">
+      <c r="G22" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H22" s="19" t="s">
+      <c r="H22" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="34" t="s">
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="27" t="s">
         <v>44</v>
       </c>
       <c r="N22" s="5"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="52" t="s">
+      <c r="R22" s="61" t="s">
         <v>73</v>
       </c>
-      <c r="S22" s="53"/>
-      <c r="T22" s="53"/>
-      <c r="U22" s="53"/>
-      <c r="V22" s="54"/>
-      <c r="W22" s="6"/>
-      <c r="X22" s="6"/>
-      <c r="Y22" s="6"/>
-      <c r="Z22" s="6"/>
-      <c r="AA22" s="6"/>
-      <c r="AB22" s="6"/>
-      <c r="AC22" s="6"/>
-      <c r="AD22" s="52" t="s">
+      <c r="S22" s="62"/>
+      <c r="T22" s="62"/>
+      <c r="U22" s="62"/>
+      <c r="V22" s="63"/>
+      <c r="AD22" s="61" t="s">
         <v>74</v>
       </c>
-      <c r="AE22" s="53"/>
-      <c r="AF22" s="53"/>
-      <c r="AG22" s="53"/>
-      <c r="AH22" s="54"/>
-      <c r="AI22" s="6"/>
-      <c r="AJ22" s="6"/>
-      <c r="AK22" s="6"/>
-      <c r="AL22" s="7"/>
+      <c r="AE22" s="62"/>
+      <c r="AF22" s="62"/>
+      <c r="AG22" s="62"/>
+      <c r="AH22" s="63"/>
+      <c r="AL22" s="6"/>
     </row>
     <row r="23" spans="2:38" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
+      <c r="E23" s="6"/>
       <c r="F23" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="G23" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H23" s="19" t="s">
+      <c r="H23" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
       <c r="M23" s="2"/>
       <c r="N23" s="5"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="55"/>
-      <c r="S23" s="56"/>
-      <c r="T23" s="56"/>
-      <c r="U23" s="56"/>
-      <c r="V23" s="57"/>
-      <c r="W23" s="6"/>
-      <c r="X23" s="6"/>
-      <c r="Y23" s="6"/>
-      <c r="Z23" s="6"/>
-      <c r="AA23" s="6"/>
-      <c r="AB23" s="6"/>
-      <c r="AC23" s="6"/>
-      <c r="AD23" s="55"/>
-      <c r="AE23" s="56"/>
-      <c r="AF23" s="56"/>
-      <c r="AG23" s="56"/>
-      <c r="AH23" s="57"/>
-      <c r="AI23" s="6"/>
-      <c r="AJ23" s="6"/>
-      <c r="AK23" s="6"/>
-      <c r="AL23" s="7"/>
+      <c r="R23" s="64"/>
+      <c r="S23" s="65"/>
+      <c r="T23" s="65"/>
+      <c r="U23" s="65"/>
+      <c r="V23" s="66"/>
+      <c r="AD23" s="64"/>
+      <c r="AE23" s="65"/>
+      <c r="AF23" s="65"/>
+      <c r="AG23" s="65"/>
+      <c r="AH23" s="66"/>
+      <c r="AL23" s="6"/>
     </row>
     <row r="24" spans="2:38" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="5"/>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
+      <c r="E24" s="6"/>
       <c r="F24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G24" s="19" t="s">
+      <c r="G24" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H24" s="19" t="s">
+      <c r="H24" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19" t="s">
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18" t="s">
         <v>33</v>
       </c>
       <c r="M24" s="4"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
-      <c r="S24" s="9"/>
-      <c r="T24" s="9"/>
-      <c r="U24" s="9"/>
-      <c r="V24" s="9"/>
-      <c r="W24" s="9"/>
-      <c r="X24" s="9"/>
-      <c r="Y24" s="9"/>
-      <c r="Z24" s="9"/>
-      <c r="AA24" s="9"/>
-      <c r="AB24" s="9"/>
-      <c r="AC24" s="9"/>
-      <c r="AD24" s="9"/>
-      <c r="AE24" s="9"/>
-      <c r="AF24" s="9"/>
-      <c r="AG24" s="9"/>
-      <c r="AH24" s="9"/>
-      <c r="AI24" s="9"/>
-      <c r="AJ24" s="9"/>
-      <c r="AK24" s="9"/>
-      <c r="AL24" s="10"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="8"/>
+      <c r="U24" s="8"/>
+      <c r="V24" s="8"/>
+      <c r="W24" s="8"/>
+      <c r="X24" s="8"/>
+      <c r="Y24" s="8"/>
+      <c r="Z24" s="8"/>
+      <c r="AA24" s="8"/>
+      <c r="AB24" s="8"/>
+      <c r="AC24" s="8"/>
+      <c r="AD24" s="8"/>
+      <c r="AE24" s="8"/>
+      <c r="AF24" s="8"/>
+      <c r="AG24" s="8"/>
+      <c r="AH24" s="8"/>
+      <c r="AI24" s="8"/>
+      <c r="AJ24" s="8"/>
+      <c r="AK24" s="8"/>
+      <c r="AL24" s="9"/>
     </row>
     <row r="25" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B25" s="5"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="7"/>
+      <c r="E25" s="6"/>
       <c r="F25" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G25" s="19" t="s">
+      <c r="G25" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H25" s="19" t="s">
+      <c r="H25" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
       <c r="M25" s="4"/>
     </row>
     <row r="26" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B26" s="5"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E26" s="7"/>
+      <c r="E26" s="6"/>
       <c r="F26" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G26" s="19" t="s">
+      <c r="G26" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H26" s="19" t="s">
+      <c r="H26" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
       <c r="M26" s="2"/>
     </row>
     <row r="27" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B27" s="5"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="7"/>
+      <c r="E27" s="6"/>
       <c r="F27" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G27" s="19" t="s">
+      <c r="G27" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H27" s="19" t="s">
+      <c r="H27" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
       <c r="M27" s="2"/>
     </row>
     <row r="28" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B28" s="5"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="7"/>
+      <c r="E28" s="6"/>
       <c r="F28" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G28" s="19" t="s">
+      <c r="G28" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H28" s="19" t="s">
+      <c r="H28" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
       <c r="M28" s="2"/>
     </row>
     <row r="29" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B29" s="5"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E29" s="7"/>
+      <c r="E29" s="6"/>
       <c r="F29" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G29" s="19" t="s">
+      <c r="G29" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H29" s="19" t="s">
+      <c r="H29" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
       <c r="M29" s="2"/>
     </row>
     <row r="30" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B30" s="5"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E30" s="7"/>
+      <c r="E30" s="6"/>
       <c r="F30" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G30" s="19" t="s">
+      <c r="G30" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H30" s="19" t="s">
+      <c r="H30" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
       <c r="M30" s="2"/>
     </row>
     <row r="31" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B31" s="5"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E31" s="7"/>
+      <c r="E31" s="6"/>
       <c r="F31" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G31" s="19" t="s">
+      <c r="G31" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H31" s="19" t="s">
+      <c r="H31" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
       <c r="M31" s="2"/>
     </row>
     <row r="32" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B32" s="5"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="7"/>
+      <c r="E32" s="6"/>
       <c r="F32" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G32" s="19" t="s">
+      <c r="G32" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H32" s="19" t="s">
+      <c r="H32" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
       <c r="M32" s="2"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B33" s="5"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E33" s="7"/>
+      <c r="E33" s="6"/>
       <c r="F33" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G33" s="19" t="s">
+      <c r="G33" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="H33" s="19" t="s">
+      <c r="H33" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
       <c r="M33" s="2"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B34" s="5"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E34" s="7"/>
+      <c r="E34" s="6"/>
       <c r="F34" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G34" s="19" t="s">
+      <c r="G34" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H34" s="19" t="s">
+      <c r="H34" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B35" s="5"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="7" t="s">
+      <c r="E35" s="6" t="s">
         <v>17</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G35" s="19" t="s">
+      <c r="G35" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H35" s="19" t="s">
+      <c r="H35" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
-      <c r="L35" s="19"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B36" s="5"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="7" t="s">
+      <c r="E36" s="6" t="s">
         <v>18</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G36" s="19" t="s">
+      <c r="G36" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H36" s="19" t="s">
+      <c r="H36" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="19"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
     </row>
     <row r="37" spans="2:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="8"/>
-      <c r="C37" s="9" t="s">
+      <c r="B37" s="7"/>
+      <c r="C37" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D37" s="9"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="8" t="s">
+      <c r="D37" s="8"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G37" s="20" t="s">
+      <c r="G37" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="H37" s="20" t="s">
+      <c r="H37" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="20"/>
-      <c r="L37" s="20"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="19"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
@@ -4160,11 +3985,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="O17:S17"/>
-    <mergeCell ref="U17:Y17"/>
-    <mergeCell ref="AA17:AE17"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="O6:V6"/>
+    <mergeCell ref="N2:AL2"/>
+    <mergeCell ref="AG11:AK11"/>
+    <mergeCell ref="AA9:AE9"/>
+    <mergeCell ref="AG9:AK9"/>
+    <mergeCell ref="X6:Z6"/>
+    <mergeCell ref="O9:S9"/>
+    <mergeCell ref="U9:Y9"/>
+    <mergeCell ref="O11:S11"/>
+    <mergeCell ref="U11:Y11"/>
     <mergeCell ref="R22:V23"/>
     <mergeCell ref="AD22:AH23"/>
     <mergeCell ref="O19:Y19"/>
@@ -4175,19 +4007,12 @@
     <mergeCell ref="U15:Y15"/>
     <mergeCell ref="AA15:AE15"/>
     <mergeCell ref="AG15:AK15"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="O17:S17"/>
+    <mergeCell ref="U17:Y17"/>
+    <mergeCell ref="AA17:AE17"/>
     <mergeCell ref="AA11:AE11"/>
-    <mergeCell ref="AG11:AK11"/>
-    <mergeCell ref="AA9:AE9"/>
-    <mergeCell ref="AG9:AK9"/>
-    <mergeCell ref="X6:Z6"/>
-    <mergeCell ref="O9:S9"/>
-    <mergeCell ref="U9:Y9"/>
-    <mergeCell ref="O11:S11"/>
-    <mergeCell ref="U11:Y11"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="O6:V6"/>
-    <mergeCell ref="N2:AL2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4213,179 +4038,179 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:5" s="62" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="21" t="s">
+    <row r="2" spans="2:5" s="40" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="23"/>
-    </row>
-    <row r="3" spans="2:5" s="25" customFormat="1" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="63" t="s">
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="75"/>
+    </row>
+    <row r="3" spans="2:5" s="21" customFormat="1" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="C3" s="64" t="s">
+      <c r="C3" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="D3" s="64" t="s">
+      <c r="D3" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="43" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="78" x14ac:dyDescent="0.3">
-      <c r="B4" s="68">
+      <c r="B4" s="46">
         <v>1</v>
       </c>
-      <c r="C4" s="69" t="s">
+      <c r="C4" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="D4" s="69" t="s">
+      <c r="D4" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="E4" s="66" t="s">
+      <c r="E4" s="44" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="78" x14ac:dyDescent="0.3">
-      <c r="B5" s="68">
+      <c r="B5" s="46">
         <v>2</v>
       </c>
-      <c r="C5" s="69" t="s">
+      <c r="C5" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="D5" s="69" t="s">
+      <c r="D5" s="47" t="s">
         <v>122</v>
       </c>
-      <c r="E5" s="66" t="s">
+      <c r="E5" s="44" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="68">
+      <c r="B6" s="46">
         <v>3</v>
       </c>
-      <c r="C6" s="69" t="s">
+      <c r="C6" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="69" t="s">
+      <c r="D6" s="47" t="s">
         <v>116</v>
       </c>
-      <c r="E6" s="66" t="s">
+      <c r="E6" s="44" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B7" s="68">
+      <c r="B7" s="46">
         <v>4</v>
       </c>
-      <c r="C7" s="69" t="s">
+      <c r="C7" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="D7" s="69" t="s">
+      <c r="D7" s="47" t="s">
         <v>125</v>
       </c>
-      <c r="E7" s="66" t="s">
+      <c r="E7" s="44" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B8" s="68">
+      <c r="B8" s="46">
         <v>5</v>
       </c>
-      <c r="C8" s="69" t="s">
+      <c r="C8" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="D8" s="69" t="s">
+      <c r="D8" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="E8" s="66" t="s">
+      <c r="E8" s="44" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B9" s="68">
+      <c r="B9" s="46">
         <v>6</v>
       </c>
-      <c r="C9" s="69" t="s">
+      <c r="C9" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="D9" s="69" t="s">
+      <c r="D9" s="47" t="s">
         <v>117</v>
       </c>
-      <c r="E9" s="66" t="s">
+      <c r="E9" s="44" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B10" s="68">
+      <c r="B10" s="46">
         <v>7</v>
       </c>
-      <c r="C10" s="69" t="s">
+      <c r="C10" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="D10" s="69" t="s">
+      <c r="D10" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="E10" s="66" t="s">
+      <c r="E10" s="44" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="68">
+      <c r="B11" s="46">
         <v>8</v>
       </c>
-      <c r="C11" s="69" t="s">
+      <c r="C11" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="D11" s="69" t="s">
+      <c r="D11" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="E11" s="66" t="s">
+      <c r="E11" s="44" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="68">
+      <c r="B12" s="46">
         <v>9</v>
       </c>
-      <c r="C12" s="69" t="s">
+      <c r="C12" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="D12" s="69" t="s">
+      <c r="D12" s="47" t="s">
         <v>119</v>
       </c>
-      <c r="E12" s="66" t="s">
+      <c r="E12" s="44" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="68">
+      <c r="B13" s="46">
         <v>10</v>
       </c>
-      <c r="C13" s="69" t="s">
+      <c r="C13" s="47" t="s">
         <v>113</v>
       </c>
-      <c r="D13" s="69" t="s">
+      <c r="D13" s="47" t="s">
         <v>120</v>
       </c>
-      <c r="E13" s="66" t="s">
+      <c r="E13" s="44" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="70">
+      <c r="B14" s="48">
         <v>11</v>
       </c>
-      <c r="C14" s="71" t="s">
+      <c r="C14" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="D14" s="71" t="s">
+      <c r="D14" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="E14" s="67" t="s">
+      <c r="E14" s="45" t="s">
         <v>140</v>
       </c>
     </row>
@@ -4401,7 +4226,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36C30BBA-9A41-44E0-BD01-C1FC88260213}">
   <dimension ref="B2:X77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
@@ -4442,7 +4267,7 @@
       </c>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="L5" s="72" t="s">
+      <c r="L5" s="50" t="s">
         <v>6</v>
       </c>
       <c r="S5" s="1" t="s">
@@ -4476,12 +4301,11 @@
       <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="L7" s="73" t="s">
+      <c r="L7" s="51" t="s">
         <v>192</v>
       </c>
       <c r="O7"/>
-      <c r="P7" s="76" t="s">
+      <c r="P7" s="54" t="s">
         <v>150</v>
       </c>
       <c r="Q7"/>
@@ -4489,61 +4313,61 @@
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B8" s="5"/>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L8" s="74" t="s">
+      <c r="L8" s="52" t="s">
         <v>8</v>
       </c>
       <c r="O8"/>
       <c r="P8"/>
-      <c r="Q8" s="76" t="s">
+      <c r="Q8" s="54" t="s">
         <v>243</v>
       </c>
       <c r="R8"/>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B9" s="5"/>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L9" s="74" t="s">
+      <c r="L9" s="52" t="s">
         <v>9</v>
       </c>
       <c r="O9"/>
       <c r="P9"/>
       <c r="Q9"/>
-      <c r="R9" s="76" t="s">
+      <c r="R9" s="54" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B10" s="5"/>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L10" s="73" t="s">
+      <c r="L10" s="51" t="s">
         <v>193</v>
       </c>
       <c r="O10"/>
       <c r="P10"/>
       <c r="Q10"/>
-      <c r="R10" s="76" t="s">
+      <c r="R10" s="54" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B11" s="5"/>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L11" s="73" t="s">
+      <c r="L11" s="51" t="s">
         <v>194</v>
       </c>
       <c r="O11"/>
       <c r="P11"/>
       <c r="Q11"/>
-      <c r="R11" s="76" t="s">
+      <c r="R11" s="54" t="s">
         <v>148</v>
       </c>
     </row>
@@ -4551,29 +4375,29 @@
       <c r="B12" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="L12" s="73" t="s">
+      <c r="L12" s="51" t="s">
         <v>195</v>
       </c>
       <c r="O12"/>
       <c r="P12"/>
       <c r="Q12"/>
-      <c r="R12" s="76" t="s">
+      <c r="R12" s="54" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="L13" s="73" t="s">
+      <c r="L13" s="51" t="s">
         <v>196</v>
       </c>
       <c r="O13"/>
       <c r="P13"/>
       <c r="Q13"/>
-      <c r="R13" s="76" t="s">
+      <c r="R13" s="54" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="L14" s="73" t="s">
+      <c r="L14" s="51" t="s">
         <v>197</v>
       </c>
     </row>
@@ -4581,7 +4405,7 @@
       <c r="B15" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="L15" s="73" t="s">
+      <c r="L15" s="51" t="s">
         <v>198</v>
       </c>
     </row>
@@ -4592,7 +4416,7 @@
       <c r="D16" s="1">
         <v>0</v>
       </c>
-      <c r="L16" s="73" t="s">
+      <c r="L16" s="51" t="s">
         <v>199</v>
       </c>
     </row>
@@ -4600,7 +4424,7 @@
       <c r="E17" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="L17" s="73" t="s">
+      <c r="L17" s="51" t="s">
         <v>200</v>
       </c>
     </row>
@@ -4608,7 +4432,7 @@
       <c r="F18" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="L18" s="72" t="s">
+      <c r="L18" s="50" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4624,7 +4448,7 @@
       <c r="F20" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="L20" s="72" t="s">
+      <c r="L20" s="50" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4632,7 +4456,7 @@
       <c r="F21" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="L21" s="73" t="s">
+      <c r="L21" s="51" t="s">
         <v>202</v>
       </c>
     </row>
@@ -4640,7 +4464,7 @@
       <c r="F22" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="L22" s="72" t="s">
+      <c r="L22" s="50" t="s">
         <v>203</v>
       </c>
     </row>
@@ -4648,7 +4472,7 @@
       <c r="G23" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L23" s="75" t="s">
+      <c r="L23" s="53" t="s">
         <v>204</v>
       </c>
     </row>
@@ -4656,7 +4480,7 @@
       <c r="G24" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="L24" s="72" t="s">
+      <c r="L24" s="50" t="s">
         <v>203</v>
       </c>
     </row>
@@ -4664,7 +4488,7 @@
       <c r="G25" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="L25" s="75" t="s">
+      <c r="L25" s="53" t="s">
         <v>205</v>
       </c>
     </row>
@@ -4672,7 +4496,7 @@
       <c r="G26" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="L26" s="73" t="s">
+      <c r="L26" s="51" t="s">
         <v>206</v>
       </c>
     </row>
@@ -4680,7 +4504,7 @@
       <c r="F27" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L27" s="73" t="s">
+      <c r="L27" s="51" t="s">
         <v>207</v>
       </c>
     </row>
@@ -4688,7 +4512,7 @@
       <c r="E28" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="L28" s="72" t="s">
+      <c r="L28" s="50" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4704,7 +4528,7 @@
       <c r="G30" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="L30" s="73" t="s">
+      <c r="L30" s="51" t="s">
         <v>209</v>
       </c>
     </row>
@@ -4712,7 +4536,7 @@
       <c r="H31" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="L31" s="72" t="s">
+      <c r="L31" s="50" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4720,7 +4544,7 @@
       <c r="H32" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="L32" s="73" t="s">
+      <c r="L32" s="51" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4728,7 +4552,7 @@
       <c r="H33" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="L33" s="75" t="s">
+      <c r="L33" s="53" t="s">
         <v>210</v>
       </c>
     </row>
@@ -4736,7 +4560,7 @@
       <c r="G34" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="L34" s="75" t="s">
+      <c r="L34" s="53" t="s">
         <v>211</v>
       </c>
     </row>
@@ -4744,7 +4568,7 @@
       <c r="H35" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="L35" s="75" t="s">
+      <c r="L35" s="53" t="s">
         <v>212</v>
       </c>
     </row>
@@ -4752,7 +4576,7 @@
       <c r="G36" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="L36" s="75" t="s">
+      <c r="L36" s="53" t="s">
         <v>213</v>
       </c>
     </row>
@@ -4760,7 +4584,7 @@
       <c r="H37" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="L37" s="75" t="s">
+      <c r="L37" s="53" t="s">
         <v>214</v>
       </c>
     </row>
@@ -4768,7 +4592,7 @@
       <c r="H38" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="L38" s="75" t="s">
+      <c r="L38" s="53" t="s">
         <v>215</v>
       </c>
     </row>
@@ -4776,7 +4600,7 @@
       <c r="H39" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L39" s="72" t="s">
+      <c r="L39" s="50" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4784,7 +4608,7 @@
       <c r="G40" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="L40" s="73" t="s">
+      <c r="L40" s="51" t="s">
         <v>216</v>
       </c>
     </row>
@@ -4792,7 +4616,7 @@
       <c r="H41" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="L41" s="75" t="s">
+      <c r="L41" s="53" t="s">
         <v>213</v>
       </c>
     </row>
@@ -4800,7 +4624,7 @@
       <c r="H42" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="L42" s="75" t="s">
+      <c r="L42" s="53" t="s">
         <v>217</v>
       </c>
     </row>
@@ -4808,7 +4632,7 @@
       <c r="G43" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="L43" s="75" t="s">
+      <c r="L43" s="53" t="s">
         <v>218</v>
       </c>
     </row>
@@ -4816,7 +4640,7 @@
       <c r="H44" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="L44" s="75" t="s">
+      <c r="L44" s="53" t="s">
         <v>219</v>
       </c>
     </row>
@@ -4824,7 +4648,7 @@
       <c r="H45" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="L45" s="73" t="s">
+      <c r="L45" s="51" t="s">
         <v>220</v>
       </c>
     </row>
@@ -4832,7 +4656,7 @@
       <c r="H46" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="L46" s="72" t="s">
+      <c r="L46" s="50" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4840,7 +4664,7 @@
       <c r="H47" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="L47" s="73" t="s">
+      <c r="L47" s="51" t="s">
         <v>221</v>
       </c>
     </row>
@@ -4848,7 +4672,7 @@
       <c r="G48" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="L48" s="75" t="s">
+      <c r="L48" s="53" t="s">
         <v>222</v>
       </c>
     </row>
@@ -4856,7 +4680,7 @@
       <c r="H49" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="L49" s="75" t="s">
+      <c r="L49" s="53" t="s">
         <v>223</v>
       </c>
     </row>
@@ -4864,7 +4688,7 @@
       <c r="H50" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="L50" s="75" t="s">
+      <c r="L50" s="53" t="s">
         <v>213</v>
       </c>
     </row>
@@ -4872,7 +4696,7 @@
       <c r="G51" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="L51" s="75" t="s">
+      <c r="L51" s="53" t="s">
         <v>214</v>
       </c>
     </row>
@@ -4888,7 +4712,7 @@
       <c r="H53" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="L53" s="72" t="s">
+      <c r="L53" s="50" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4904,7 +4728,7 @@
       <c r="H55" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="L55" s="73" t="s">
+      <c r="L55" s="51" t="s">
         <v>225</v>
       </c>
     </row>
@@ -4912,7 +4736,7 @@
       <c r="G56" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="L56" s="73" t="s">
+      <c r="L56" s="51" t="s">
         <v>226</v>
       </c>
     </row>
@@ -4922,7 +4746,7 @@
       </c>
     </row>
     <row r="58" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="L58" s="72" t="s">
+      <c r="L58" s="50" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4932,32 +4756,32 @@
       </c>
     </row>
     <row r="60" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="L60" s="73" t="s">
+      <c r="L60" s="51" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="61" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="L61" s="73" t="s">
+      <c r="L61" s="51" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="62" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="L62" s="73" t="s">
+      <c r="L62" s="51" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="63" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="L63" s="73" t="s">
+      <c r="L63" s="51" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="64" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="L64" s="73" t="s">
+      <c r="L64" s="51" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="65" spans="12:12" x14ac:dyDescent="0.3">
-      <c r="L65" s="73" t="s">
+      <c r="L65" s="51" t="s">
         <v>233</v>
       </c>
     </row>
@@ -4972,7 +4796,7 @@
       </c>
     </row>
     <row r="68" spans="12:12" x14ac:dyDescent="0.3">
-      <c r="L68" s="72" t="s">
+      <c r="L68" s="50" t="s">
         <v>6</v>
       </c>
     </row>
@@ -5054,248 +4878,248 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:45" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C2" s="76" t="s">
+      <c r="C2" s="54" t="s">
         <v>259</v>
       </c>
-      <c r="N2" s="76" t="s">
+      <c r="N2" s="54" t="s">
         <v>261</v>
       </c>
-      <c r="W2" s="76" t="s">
+      <c r="W2" s="54" t="s">
         <v>263</v>
       </c>
-      <c r="AF2" s="76" t="s">
+      <c r="AF2" s="54" t="s">
         <v>265</v>
       </c>
-      <c r="AP2" s="76" t="s">
+      <c r="AP2" s="54" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="3" spans="3:45" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D3" s="76" t="s">
+      <c r="D3" s="54" t="s">
         <v>243</v>
       </c>
-      <c r="O3" s="76" t="s">
+      <c r="O3" s="54" t="s">
         <v>243</v>
       </c>
-      <c r="X3" s="76" t="s">
+      <c r="X3" s="54" t="s">
         <v>243</v>
       </c>
-      <c r="AG3" s="76" t="s">
+      <c r="AG3" s="54" t="s">
         <v>243</v>
       </c>
-      <c r="AQ3" s="76" t="s">
+      <c r="AQ3" s="54" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="4" spans="3:45" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E4" s="76" t="s">
+      <c r="E4" s="54" t="s">
         <v>260</v>
       </c>
-      <c r="P4" s="76" t="s">
+      <c r="P4" s="54" t="s">
         <v>262</v>
       </c>
-      <c r="Y4" s="76" t="s">
+      <c r="Y4" s="54" t="s">
         <v>264</v>
       </c>
-      <c r="AH4" s="76" t="s">
+      <c r="AH4" s="54" t="s">
         <v>266</v>
       </c>
-      <c r="AR4" s="76" t="s">
+      <c r="AR4" s="54" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="5" spans="3:45" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E5" s="76" t="s">
+      <c r="E5" s="54" t="s">
         <v>244</v>
       </c>
-      <c r="P5" s="76" t="s">
+      <c r="P5" s="54" t="s">
         <v>244</v>
       </c>
-      <c r="Y5" s="76" t="s">
+      <c r="Y5" s="54" t="s">
         <v>244</v>
       </c>
-      <c r="AH5" s="76" t="s">
+      <c r="AH5" s="54" t="s">
         <v>244</v>
       </c>
-      <c r="AR5" s="76" t="s">
+      <c r="AR5" s="54" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="6" spans="3:45" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E6" s="76" t="s">
+      <c r="E6" s="54" t="s">
         <v>245</v>
       </c>
-      <c r="P6" s="76" t="s">
+      <c r="P6" s="54" t="s">
         <v>245</v>
       </c>
-      <c r="Y6" s="76" t="s">
+      <c r="Y6" s="54" t="s">
         <v>245</v>
       </c>
-      <c r="AH6" s="76" t="s">
+      <c r="AH6" s="54" t="s">
         <v>245</v>
       </c>
-      <c r="AR6" s="76" t="s">
+      <c r="AR6" s="54" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="7" spans="3:45" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E7" s="76" t="s">
+      <c r="E7" s="54" t="s">
         <v>246</v>
       </c>
-      <c r="P7" s="76" t="s">
+      <c r="P7" s="54" t="s">
         <v>246</v>
       </c>
-      <c r="Y7" s="76" t="s">
+      <c r="Y7" s="54" t="s">
         <v>246</v>
       </c>
-      <c r="AH7" s="76" t="s">
+      <c r="AH7" s="54" t="s">
         <v>246</v>
       </c>
-      <c r="AR7" s="76" t="s">
+      <c r="AR7" s="54" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="8" spans="3:45" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E8" s="76" t="s">
+      <c r="E8" s="54" t="s">
         <v>259</v>
       </c>
-      <c r="P8" s="76" t="s">
+      <c r="P8" s="54" t="s">
         <v>261</v>
       </c>
-      <c r="Y8" s="76" t="s">
+      <c r="Y8" s="54" t="s">
         <v>263</v>
       </c>
-      <c r="AH8" s="76" t="s">
+      <c r="AH8" s="54" t="s">
         <v>265</v>
       </c>
-      <c r="AR8" s="76" t="s">
+      <c r="AR8" s="54" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="9" spans="3:45" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="F9" s="76" t="s">
+      <c r="F9" s="54" t="s">
         <v>247</v>
       </c>
-      <c r="Q9" s="76" t="s">
+      <c r="Q9" s="54" t="s">
         <v>247</v>
       </c>
-      <c r="Z9" s="76" t="s">
+      <c r="Z9" s="54" t="s">
         <v>247</v>
       </c>
-      <c r="AI9" s="76" t="s">
+      <c r="AI9" s="54" t="s">
         <v>151</v>
       </c>
-      <c r="AS9" s="76" t="s">
+      <c r="AS9" s="54" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="10" spans="3:45" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="F10" s="76" t="s">
+      <c r="F10" s="54" t="s">
         <v>248</v>
       </c>
-      <c r="Q10" s="76" t="s">
+      <c r="Q10" s="54" t="s">
         <v>248</v>
       </c>
-      <c r="Z10" s="76" t="s">
+      <c r="Z10" s="54" t="s">
         <v>248</v>
       </c>
-      <c r="AI10" s="76" t="s">
+      <c r="AI10" s="54" t="s">
         <v>251</v>
       </c>
-      <c r="AS10" s="76" t="s">
+      <c r="AS10" s="54" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="11" spans="3:45" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="F11" s="76" t="s">
+      <c r="F11" s="54" t="s">
         <v>249</v>
       </c>
-      <c r="Q11" s="76" t="s">
+      <c r="Q11" s="54" t="s">
         <v>252</v>
       </c>
-      <c r="Y11" s="76" t="s">
+      <c r="Y11" s="54" t="s">
         <v>153</v>
       </c>
-      <c r="AI11" s="76" t="s">
+      <c r="AI11" s="54" t="s">
         <v>257</v>
       </c>
-      <c r="AS11" s="76" t="s">
+      <c r="AS11" s="54" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="12" spans="3:45" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="F12" s="76" t="s">
+      <c r="F12" s="54" t="s">
         <v>250</v>
       </c>
-      <c r="P12" s="76" t="s">
+      <c r="P12" s="54" t="s">
         <v>153</v>
       </c>
-      <c r="X12" s="76" t="s">
+      <c r="X12" s="54" t="s">
         <v>153</v>
       </c>
-      <c r="AI12" s="76" t="s">
+      <c r="AI12" s="54" t="s">
         <v>253</v>
       </c>
-      <c r="AR12" s="76" t="s">
+      <c r="AR12" s="54" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="13" spans="3:45" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E13" s="76" t="s">
+      <c r="E13" s="54" t="s">
         <v>153</v>
       </c>
-      <c r="O13" s="76" t="s">
+      <c r="O13" s="54" t="s">
         <v>153</v>
       </c>
-      <c r="W13" s="76" t="s">
+      <c r="W13" s="54" t="s">
         <v>153</v>
       </c>
-      <c r="AJ13" s="76" t="s">
+      <c r="AJ13" s="54" t="s">
         <v>254</v>
       </c>
-      <c r="AQ13" s="76" t="s">
+      <c r="AQ13" s="54" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="14" spans="3:45" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D14" s="76" t="s">
+      <c r="D14" s="54" t="s">
         <v>153</v>
       </c>
-      <c r="N14" s="76" t="s">
+      <c r="N14" s="54" t="s">
         <v>153</v>
       </c>
-      <c r="AJ14" s="76" t="s">
+      <c r="AJ14" s="54" t="s">
         <v>255</v>
       </c>
-      <c r="AP14" s="76" t="s">
+      <c r="AP14" s="54" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="15" spans="3:45" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C15" s="76" t="s">
+      <c r="C15" s="54" t="s">
         <v>153</v>
       </c>
-      <c r="AJ15" s="76" t="s">
+      <c r="AJ15" s="54" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="16" spans="3:45" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="AI16" s="76" t="s">
+      <c r="AI16" s="54" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="17" spans="32:34" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="AH17" s="76" t="s">
+      <c r="AH17" s="54" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="18" spans="32:34" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="AG18" s="76" t="s">
+      <c r="AG18" s="54" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="19" spans="32:34" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="AF19" s="76" t="s">
+      <c r="AF19" s="54" t="s">
         <v>153</v>
       </c>
     </row>
@@ -5370,4 +5194,58 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249089D0-12CB-4838-813F-FD7594184091}">
+  <dimension ref="A1:S4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E4" t="s">
+        <v>271</v>
+      </c>
+      <c r="G4" t="s">
+        <v>272</v>
+      </c>
+      <c r="I4" t="s">
+        <v>273</v>
+      </c>
+      <c r="K4" t="s">
+        <v>274</v>
+      </c>
+      <c r="M4" t="s">
+        <v>275</v>
+      </c>
+      <c r="O4" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>277</v>
+      </c>
+      <c r="S4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>